<commit_message>
updated MFA system solution
</commit_message>
<xml_diff>
--- a/data/Carbon_Footprint_Primary.xlsx
+++ b/data/Carbon_Footprint_Primary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3B707C-B928-4F4B-B810-18F06CF76EFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691F6199-2CCC-4E2E-AC13-EF697666A7A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{14E8540C-EDEE-4050-9B8C-8C7F8EC6EA2C}"/>
   </bookViews>
@@ -207,9 +207,6 @@
     <t>ODYM_Classifications_Master_Al_cars</t>
   </si>
   <si>
-    <t>Scenario</t>
-  </si>
-  <si>
     <t>Baseline</t>
   </si>
   <si>
@@ -234,7 +231,10 @@
     <t>Romain Billy</t>
   </si>
   <si>
-    <t>Carbon footprint of primary aluminium production</t>
+    <t>Carbon_Footprint_Scenario</t>
+  </si>
+  <si>
+    <t>Scenarios for carbon footprint of Al production</t>
   </si>
 </sst>
 </file>
@@ -309,9 +309,18 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -322,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -340,6 +349,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -658,7 +668,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +723,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -835,7 +845,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -904,7 +914,7 @@
         <v>33</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1065,22 +1075,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>51</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>1</v>
@@ -1155,7 +1165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B481CB-FC39-456D-A965-38066FA722C2}">
   <dimension ref="A1:DJ152"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F152"/>
     </sheetView>
   </sheetViews>
@@ -1163,19 +1173,19 @@
   <sheetData>
     <row r="1" spans="1:114" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:114" x14ac:dyDescent="0.25">

</xml_diff>